<commit_message>
Minor PCB and parts list update
</commit_message>
<xml_diff>
--- a/mechanics/V1INV/STLs/Parts List.xlsx
+++ b/mechanics/V1INV/STLs/Parts List.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Part Name</t>
   </si>
@@ -168,19 +168,19 @@
     <t>Volume (cm^3)</t>
   </si>
   <si>
-    <t>g/cm^3</t>
-  </si>
-  <si>
-    <t>(ABS) Density</t>
-  </si>
-  <si>
     <t>Totals</t>
   </si>
   <si>
     <t>Volume subtotal</t>
   </si>
   <si>
-    <t>Overall Mass (ABS)</t>
+    <t>Material/Process</t>
+  </si>
+  <si>
+    <t>Nylon/SLS</t>
+  </si>
+  <si>
+    <t>ASA/FDM</t>
   </si>
 </sst>
 </file>
@@ -190,19 +190,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
     </font>
     <font>
       <b/>
@@ -246,12 +240,12 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,20 +560,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E684A401-D1C1-4639-87EE-CCEF01DE4432}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.5546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.21875" style="4" customWidth="1"/>
-    <col min="4" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="20" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="6" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="20" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="16.2" x14ac:dyDescent="0.35">
@@ -589,703 +583,822 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>2</v>
       </c>
       <c r="C2" s="4">
         <v>14.804</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <f>B2*C2</f>
         <v>29.608000000000001</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="6">
-        <v>1.06</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>24.797999999999998</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <f t="shared" ref="D3:D45" si="0">B3*C3</f>
         <v>24.797999999999998</v>
       </c>
+      <c r="G3" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="4">
         <v>1.369</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>1.369</v>
       </c>
+      <c r="G4" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="4">
         <v>0.38100000000000001</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>3.048</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
         <v>2</v>
       </c>
       <c r="C6" s="4">
         <v>13.702</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>27.404</v>
       </c>
+      <c r="G6" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
       <c r="C7" s="4">
         <v>88.796000000000006</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>88.796000000000006</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="4">
         <v>3.641</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>3.641</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
       <c r="C9" s="4">
         <v>28.925999999999998</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>28.925999999999998</v>
       </c>
+      <c r="G9" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="4">
         <v>28.925999999999998</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>28.925999999999998</v>
       </c>
+      <c r="G10" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="3">
         <v>6</v>
       </c>
       <c r="C11" s="4">
         <v>30.643999999999998</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>183.86399999999998</v>
       </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12" s="4">
         <v>40.381</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>40.381</v>
       </c>
+      <c r="G12" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13" s="4">
         <v>9.9510000000000005</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>29.853000000000002</v>
       </c>
+      <c r="G13" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="3">
         <v>3</v>
       </c>
       <c r="C14" s="4">
         <v>3.9470000000000001</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>11.841000000000001</v>
       </c>
+      <c r="G14" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>1</v>
       </c>
       <c r="C15" s="4">
         <v>34.831000000000003</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>34.831000000000003</v>
       </c>
+      <c r="G15" s="3" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <v>12</v>
       </c>
       <c r="C16" s="4">
         <v>1.748</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>20.975999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="G16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <v>6</v>
       </c>
       <c r="C17" s="4">
         <v>4.3010000000000002</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>25.806000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="G17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="3">
         <v>3</v>
       </c>
       <c r="C18" s="4">
         <v>0.246</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <f t="shared" si="0"/>
         <v>0.73799999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="G18" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>3</v>
       </c>
       <c r="C19" s="4">
         <v>1.861</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="3">
         <f t="shared" si="0"/>
         <v>5.5830000000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="G19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>6</v>
       </c>
       <c r="C20" s="4">
         <v>11.831</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <f t="shared" si="0"/>
         <v>70.98599999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="G20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="3">
         <v>12</v>
       </c>
       <c r="C21" s="4">
         <v>0.57699999999999996</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
         <f t="shared" si="0"/>
         <v>6.9239999999999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="G21" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <v>6</v>
       </c>
       <c r="C22" s="4">
         <v>7.048</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <f t="shared" si="0"/>
         <v>42.287999999999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="G22" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="3">
         <v>4</v>
       </c>
       <c r="C23" s="4">
         <v>1.7130000000000001</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="3">
         <f t="shared" si="0"/>
         <v>6.8520000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="G23" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <v>4</v>
       </c>
       <c r="C24" s="4">
         <v>3.694</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="3">
         <f t="shared" si="0"/>
         <v>14.776</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="G24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="3">
         <v>2</v>
       </c>
       <c r="C25" s="4">
         <v>1.113</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <f t="shared" si="0"/>
         <v>2.226</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="G25" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="3">
         <v>1</v>
       </c>
       <c r="C26" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="3">
         <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="G26" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="3">
         <v>2</v>
       </c>
       <c r="C27" s="4">
         <v>9.2210000000000001</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
         <f t="shared" si="0"/>
         <v>18.442</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="G27" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="3">
         <v>2</v>
       </c>
       <c r="C28" s="4">
         <v>2.8149999999999999</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <f t="shared" si="0"/>
         <v>5.63</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="G28" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="3">
         <v>2</v>
       </c>
       <c r="C29" s="4">
         <v>11.361000000000001</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <f t="shared" si="0"/>
         <v>22.722000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="G29" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="3">
         <v>6</v>
       </c>
       <c r="C30" s="4">
         <v>2.1360000000000001</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="3">
         <f t="shared" si="0"/>
         <v>12.816000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="G30" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="3">
         <v>1</v>
       </c>
       <c r="C31" s="4">
         <v>22.917000000000002</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="3">
         <f t="shared" si="0"/>
         <v>22.917000000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="G31" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="3">
         <v>8</v>
       </c>
       <c r="C32" s="4">
         <v>4.1749999999999998</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <f t="shared" si="0"/>
         <v>33.4</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="G32" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="3">
         <v>2</v>
       </c>
       <c r="C33" s="4">
         <v>10.207000000000001</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <f t="shared" si="0"/>
         <v>20.414000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="G33" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="3">
         <v>1</v>
       </c>
       <c r="C34" s="4">
         <v>25.434999999999999</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="3">
         <f t="shared" si="0"/>
         <v>25.434999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="G34" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="3">
         <v>6</v>
       </c>
       <c r="C35" s="4">
         <v>1.6679999999999999</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <f t="shared" si="0"/>
         <v>10.007999999999999</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="G35" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="3">
         <v>1</v>
       </c>
       <c r="C36" s="4">
         <v>6.9379999999999997</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="3">
         <f t="shared" si="0"/>
         <v>6.9379999999999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="G36" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="3">
         <v>1</v>
       </c>
       <c r="C37" s="4">
         <v>11.888</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="3">
         <f t="shared" si="0"/>
         <v>11.888</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="G37" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="3">
         <v>4</v>
       </c>
       <c r="C38" s="4">
         <v>0.79700000000000004</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="3">
         <f t="shared" si="0"/>
         <v>3.1880000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="G38" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="3">
         <v>1</v>
       </c>
       <c r="C39" s="4">
         <v>4.2759999999999998</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="3">
         <f t="shared" si="0"/>
         <v>4.2759999999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="G39" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="3">
         <v>1</v>
       </c>
       <c r="C40" s="4">
         <v>4.2759999999999998</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="3">
         <f t="shared" si="0"/>
         <v>4.2759999999999998</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="G40" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="3">
         <v>1</v>
       </c>
       <c r="C41" s="4">
         <v>3.8119999999999998</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="3">
         <f t="shared" si="0"/>
         <v>3.8119999999999998</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="G41" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="3">
         <v>1</v>
       </c>
       <c r="C42" s="4">
         <v>0.67</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="3">
         <f t="shared" si="0"/>
         <v>0.67</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="G42" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="3">
         <v>2</v>
       </c>
       <c r="C43" s="4">
         <v>30.437999999999999</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="3">
         <f t="shared" si="0"/>
         <v>60.875999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="G43" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="3">
         <v>2</v>
       </c>
       <c r="C44" s="4">
         <v>2.4009999999999998</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="3">
         <f t="shared" si="0"/>
         <v>4.8019999999999996</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="G44" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="3">
         <v>1</v>
       </c>
       <c r="C45" s="4">
         <v>0.80200000000000005</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="3">
         <f t="shared" si="0"/>
         <v>0.80200000000000005</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="5">
+      <c r="G45" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="6">
         <f>SUM(B2:B45)</f>
         <v>136</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5">
-        <f t="shared" ref="C47:D47" si="1">SUM(D2:D45)</f>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6">
+        <f t="shared" ref="D47" si="1">SUM(D2:D45)</f>
         <v>1008.3029999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="2">
-        <f>D47*H2</f>
-        <v>1068.8011799999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>